<commit_message>
commit Remove Alembic migration files and update Ingredient_recette.xlsx
</commit_message>
<xml_diff>
--- a/RESSOURCES/RECETTE/Ingredient_recette.xlsx
+++ b/RESSOURCES/RECETTE/Ingredient_recette.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\econte\Desktop\Edouard\Divisio\RESSOURCES\RECETTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9505FD4-D511-445C-894C-159E6DF4E01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BFBEB6-4CB5-4EE9-8E7B-A6578A6ECA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22335" yWindow="3150" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,5 +471,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove Article model and update ProductionRecipe to include recipe_type; adjust recipe creation service to handle new field
</commit_message>
<xml_diff>
--- a/RESSOURCES/RECETTE/Ingredient_recette.xlsx
+++ b/RESSOURCES/RECETTE/Ingredient_recette.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\_apps\DIVISIO\RESSOURCES\RECETTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F4C7AF-C5C8-4380-B71F-526D948E187A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9F434A-DEFE-43E8-81D8-6B3A44AB535A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2985" windowWidth="30180" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31020" yWindow="1770" windowWidth="30180" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
     </ext>
@@ -28,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>recipe_code</t>
   </si>
@@ -45,9 +54,6 @@
     <t>is_proportional</t>
   </si>
   <si>
-    <t>REC_VACHE_BRASSE_NATURE</t>
-  </si>
-  <si>
     <t>MP_LAIT_VACHE_ENTIER</t>
   </si>
   <si>
@@ -66,13 +72,19 @@
     <t>Kg</t>
   </si>
   <si>
-    <t>REC_VACHE_BRASSE_SUCRE</t>
-  </si>
-  <si>
     <t>MPSING0001</t>
   </si>
   <si>
     <t>BASE_VACHE_BRASSE_NATURE</t>
+  </si>
+  <si>
+    <t>REC_COND_1025700</t>
+  </si>
+  <si>
+    <t>REC_PROC_BASE_VACHE_BRASSE_NATURE</t>
+  </si>
+  <si>
+    <t>REC_PROC_BASE_VACHE_BRASSE_SUCRE</t>
   </si>
 </sst>
 </file>
@@ -396,15 +408,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="48.140625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
   </cols>
   <sheetData>
@@ -427,87 +439,104 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C2">
         <v>950</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
       </c>
       <c r="C5">
         <v>940</v>
       </c>
       <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>1000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>